<commit_message>
fixed the csv file
</commit_message>
<xml_diff>
--- a/Data/Polls/federal.xlsx
+++ b/Data/Polls/federal.xlsx
@@ -110,10 +110,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -180,7 +179,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,10 +189,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -217,12 +212,12 @@
   <dimension ref="A1:I189"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G169" activeCellId="0" sqref="G169"/>
+      <selection pane="bottomLeft" activeCell="H56" activeCellId="0" sqref="H56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1685,10 +1680,10 @@
         <v>28</v>
       </c>
       <c r="H57" s="1" t="n">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I57" s="1" t="n">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,10 +1706,10 @@
         <v>22</v>
       </c>
       <c r="H58" s="1" t="n">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I58" s="1" t="n">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,10 +1729,10 @@
         <v>14</v>
       </c>
       <c r="H59" s="1" t="n">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I59" s="1" t="n">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1760,10 +1755,10 @@
         <v>7</v>
       </c>
       <c r="H60" s="1" t="n">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="I60" s="1" t="n">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1786,10 +1781,10 @@
         <v>2</v>
       </c>
       <c r="H61" s="1" t="n">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="I61" s="1" t="n">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,10 +2139,10 @@
         <v>23</v>
       </c>
       <c r="H75" s="1" t="n">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I75" s="1" t="n">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2170,10 +2165,10 @@
         <v>43</v>
       </c>
       <c r="H76" s="1" t="n">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I76" s="1" t="n">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,10 +2188,10 @@
         <v>14</v>
       </c>
       <c r="H77" s="1" t="n">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I77" s="1" t="n">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2219,10 +2214,10 @@
         <v>4</v>
       </c>
       <c r="H78" s="1" t="n">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I78" s="1" t="n">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2245,10 +2240,10 @@
         <v>1</v>
       </c>
       <c r="H79" s="1" t="n">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="I79" s="1" t="n">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2570,7 +2565,7 @@
       <c r="B92" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C92" s="3" t="n">
+      <c r="C92" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D92" s="1" t="s">
@@ -2596,7 +2591,7 @@
       <c r="B93" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C93" s="3" t="n">
+      <c r="C93" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D93" s="1" t="s">
@@ -2622,7 +2617,7 @@
       <c r="B94" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C94" s="3" t="n">
+      <c r="C94" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -2648,7 +2643,7 @@
       <c r="B95" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C95" s="3" t="n">
+      <c r="C95" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D95" s="1" t="s">
@@ -2671,7 +2666,7 @@
       <c r="B96" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C96" s="3" t="n">
+      <c r="C96" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D96" s="1" t="s">
@@ -2697,7 +2692,7 @@
       <c r="B97" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C97" s="3" t="n">
+      <c r="C97" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D97" s="1" t="s">
@@ -2723,7 +2718,7 @@
       <c r="B98" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C98" s="3" t="n">
+      <c r="C98" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -2749,7 +2744,7 @@
       <c r="B99" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C99" s="3" t="n">
+      <c r="C99" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D99" s="1" t="s">
@@ -2775,7 +2770,7 @@
       <c r="B100" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C100" s="3" t="n">
+      <c r="C100" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D100" s="1" t="s">
@@ -2801,7 +2796,7 @@
       <c r="B101" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C101" s="3" t="n">
+      <c r="C101" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -2827,7 +2822,7 @@
       <c r="B102" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C102" s="3" t="n">
+      <c r="C102" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D102" s="1" t="s">
@@ -2853,7 +2848,7 @@
       <c r="B103" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C103" s="3" t="n">
+      <c r="C103" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -2879,7 +2874,7 @@
       <c r="B104" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C104" s="3" t="n">
+      <c r="C104" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D104" s="1" t="s">
@@ -2905,7 +2900,7 @@
       <c r="B105" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C105" s="3" t="n">
+      <c r="C105" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D105" s="1" t="s">
@@ -2931,7 +2926,7 @@
       <c r="B106" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C106" s="3" t="n">
+      <c r="C106" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -2957,7 +2952,7 @@
       <c r="B107" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C107" s="3" t="n">
+      <c r="C107" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -2983,7 +2978,7 @@
       <c r="B108" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C108" s="3" t="n">
+      <c r="C108" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -3009,7 +3004,7 @@
       <c r="B109" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C109" s="3" t="n">
+      <c r="C109" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -3032,7 +3027,7 @@
       <c r="B110" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C110" s="3" t="n">
+      <c r="C110" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D110" s="1" t="s">
@@ -3058,7 +3053,7 @@
       <c r="B111" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C111" s="3" t="n">
+      <c r="C111" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D111" s="1" t="s">
@@ -3084,7 +3079,7 @@
       <c r="B112" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C112" s="3" t="n">
+      <c r="C112" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -3110,7 +3105,7 @@
       <c r="B113" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C113" s="3" t="n">
+      <c r="C113" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D113" s="1" t="s">
@@ -3136,7 +3131,7 @@
       <c r="B114" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C114" s="3" t="n">
+      <c r="C114" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D114" s="1" t="s">
@@ -3162,7 +3157,7 @@
       <c r="B115" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C115" s="3" t="n">
+      <c r="C115" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -3188,7 +3183,7 @@
       <c r="B116" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C116" s="3" t="n">
+      <c r="C116" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D116" s="1" t="s">
@@ -3211,7 +3206,7 @@
       <c r="B117" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C117" s="3" t="n">
+      <c r="C117" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -3237,7 +3232,7 @@
       <c r="B118" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C118" s="3" t="n">
+      <c r="C118" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D118" s="1" t="s">
@@ -3263,7 +3258,7 @@
       <c r="B119" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C119" s="3" t="n">
+      <c r="C119" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D119" s="1" t="s">
@@ -3289,7 +3284,7 @@
       <c r="B120" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C120" s="3" t="n">
+      <c r="C120" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -3315,7 +3310,7 @@
       <c r="B121" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C121" s="3" t="n">
+      <c r="C121" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D121" s="1" t="s">
@@ -3341,7 +3336,7 @@
       <c r="B122" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C122" s="3" t="n">
+      <c r="C122" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D122" s="1" t="s">
@@ -3367,7 +3362,7 @@
       <c r="B123" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C123" s="3" t="n">
+      <c r="C123" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D123" s="1" t="s">
@@ -3390,7 +3385,7 @@
       <c r="B124" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C124" s="3" t="n">
+      <c r="C124" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D124" s="1" t="s">
@@ -3416,7 +3411,7 @@
       <c r="B125" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C125" s="3" t="n">
+      <c r="C125" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -3442,7 +3437,7 @@
       <c r="B126" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C126" s="3" t="n">
+      <c r="C126" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D126" s="1" t="s">
@@ -3468,7 +3463,7 @@
       <c r="B127" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C127" s="3" t="n">
+      <c r="C127" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D127" s="1" t="s">
@@ -3494,7 +3489,7 @@
       <c r="B128" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C128" s="3" t="n">
+      <c r="C128" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D128" s="1" t="s">
@@ -3520,7 +3515,7 @@
       <c r="B129" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C129" s="3" t="n">
+      <c r="C129" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D129" s="1" t="s">
@@ -3546,7 +3541,7 @@
       <c r="B130" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C130" s="3" t="n">
+      <c r="C130" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D130" s="1" t="s">
@@ -3569,7 +3564,7 @@
       <c r="B131" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C131" s="3" t="n">
+      <c r="C131" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D131" s="1" t="s">
@@ -3595,7 +3590,7 @@
       <c r="B132" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C132" s="3" t="n">
+      <c r="C132" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D132" s="1" t="s">
@@ -3621,7 +3616,7 @@
       <c r="B133" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C133" s="3" t="n">
+      <c r="C133" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D133" s="1" t="s">
@@ -3647,7 +3642,7 @@
       <c r="B134" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C134" s="3" t="n">
+      <c r="C134" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D134" s="1" t="s">
@@ -3673,7 +3668,7 @@
       <c r="B135" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C135" s="3" t="n">
+      <c r="C135" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -3699,7 +3694,7 @@
       <c r="B136" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C136" s="3" t="n">
+      <c r="C136" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D136" s="1" t="s">
@@ -3725,7 +3720,7 @@
       <c r="B137" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C137" s="3" t="n">
+      <c r="C137" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D137" s="1" t="s">
@@ -3751,7 +3746,7 @@
       <c r="B138" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C138" s="3" t="n">
+      <c r="C138" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -3777,7 +3772,7 @@
       <c r="B139" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C139" s="3" t="n">
+      <c r="C139" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -3803,7 +3798,7 @@
       <c r="B140" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C140" s="3" t="n">
+      <c r="C140" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D140" s="1" t="s">
@@ -3829,7 +3824,7 @@
       <c r="B141" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C141" s="3" t="n">
+      <c r="C141" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -3855,7 +3850,7 @@
       <c r="B142" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C142" s="3" t="n">
+      <c r="C142" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D142" s="1" t="s">
@@ -3881,7 +3876,7 @@
       <c r="B143" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C143" s="3" t="n">
+      <c r="C143" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D143" s="1" t="s">
@@ -3907,7 +3902,7 @@
       <c r="B144" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C144" s="3" t="n">
+      <c r="C144" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -3933,7 +3928,7 @@
       <c r="B145" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C145" s="3" t="n">
+      <c r="C145" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D145" s="1" t="s">
@@ -3959,7 +3954,7 @@
       <c r="B146" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C146" s="3" t="n">
+      <c r="C146" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D146" s="1" t="s">
@@ -3985,7 +3980,7 @@
       <c r="B147" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C147" s="3" t="n">
+      <c r="C147" s="2" t="n">
         <v>44182</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -4011,7 +4006,7 @@
       <c r="B148" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C148" s="3" t="n">
+      <c r="C148" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D148" s="0" t="s">
@@ -4031,7 +4026,7 @@
       <c r="B149" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C149" s="3" t="n">
+      <c r="C149" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D149" s="0" t="s">
@@ -4051,7 +4046,7 @@
       <c r="B150" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C150" s="3" t="n">
+      <c r="C150" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D150" s="0" t="s">
@@ -4071,7 +4066,7 @@
       <c r="B151" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C151" s="3" t="n">
+      <c r="C151" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D151" s="0" t="s">
@@ -4088,7 +4083,7 @@
       <c r="B152" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C152" s="3" t="n">
+      <c r="C152" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D152" s="0" t="s">
@@ -4108,7 +4103,7 @@
       <c r="B153" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C153" s="3" t="n">
+      <c r="C153" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D153" s="0" t="s">
@@ -4128,7 +4123,7 @@
       <c r="B154" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C154" s="3" t="n">
+      <c r="C154" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D154" s="0" t="s">
@@ -4148,7 +4143,7 @@
       <c r="B155" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C155" s="3" t="n">
+      <c r="C155" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D155" s="0" t="s">
@@ -4168,7 +4163,7 @@
       <c r="B156" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C156" s="3" t="n">
+      <c r="C156" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D156" s="0" t="s">
@@ -4188,7 +4183,7 @@
       <c r="B157" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C157" s="3" t="n">
+      <c r="C157" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D157" s="0" t="s">
@@ -4208,7 +4203,7 @@
       <c r="B158" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C158" s="3" t="n">
+      <c r="C158" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D158" s="0" t="s">
@@ -4228,7 +4223,7 @@
       <c r="B159" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C159" s="3" t="n">
+      <c r="C159" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D159" s="0" t="s">
@@ -4248,7 +4243,7 @@
       <c r="B160" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C160" s="3" t="n">
+      <c r="C160" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D160" s="0" t="s">
@@ -4268,7 +4263,7 @@
       <c r="B161" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C161" s="3" t="n">
+      <c r="C161" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D161" s="0" t="s">
@@ -4288,7 +4283,7 @@
       <c r="B162" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C162" s="3" t="n">
+      <c r="C162" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D162" s="0" t="s">
@@ -4308,7 +4303,7 @@
       <c r="B163" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C163" s="3" t="n">
+      <c r="C163" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D163" s="0" t="s">
@@ -4325,7 +4320,7 @@
       <c r="B164" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C164" s="3" t="n">
+      <c r="C164" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D164" s="0" t="s">
@@ -4345,7 +4340,7 @@
       <c r="B165" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C165" s="3" t="n">
+      <c r="C165" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D165" s="0" t="s">
@@ -4365,7 +4360,7 @@
       <c r="B166" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C166" s="3" t="n">
+      <c r="C166" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D166" s="1" t="s">
@@ -4385,7 +4380,7 @@
       <c r="B167" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C167" s="3" t="n">
+      <c r="C167" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D167" s="1" t="s">
@@ -4405,7 +4400,7 @@
       <c r="B168" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C168" s="3" t="n">
+      <c r="C168" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D168" s="1" t="s">
@@ -4425,7 +4420,7 @@
       <c r="B169" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C169" s="3" t="n">
+      <c r="C169" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D169" s="1" t="s">
@@ -4442,7 +4437,7 @@
       <c r="B170" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C170" s="3" t="n">
+      <c r="C170" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D170" s="1" t="s">
@@ -4462,7 +4457,7 @@
       <c r="B171" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C171" s="3" t="n">
+      <c r="C171" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D171" s="1" t="s">
@@ -4482,7 +4477,7 @@
       <c r="B172" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C172" s="3" t="n">
+      <c r="C172" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D172" s="1" t="s">
@@ -4502,7 +4497,7 @@
       <c r="B173" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C173" s="3" t="n">
+      <c r="C173" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D173" s="1" t="s">
@@ -4522,7 +4517,7 @@
       <c r="B174" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C174" s="3" t="n">
+      <c r="C174" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D174" s="1" t="s">
@@ -4542,7 +4537,7 @@
       <c r="B175" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C175" s="3" t="n">
+      <c r="C175" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D175" s="1" t="s">
@@ -4559,7 +4554,7 @@
       <c r="B176" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C176" s="3" t="n">
+      <c r="C176" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D176" s="1" t="s">
@@ -4579,7 +4574,7 @@
       <c r="B177" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C177" s="3" t="n">
+      <c r="C177" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D177" s="1" t="s">
@@ -4599,7 +4594,7 @@
       <c r="B178" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C178" s="3" t="n">
+      <c r="C178" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D178" s="1" t="s">
@@ -4619,7 +4614,7 @@
       <c r="B179" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C179" s="3" t="n">
+      <c r="C179" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D179" s="1" t="s">
@@ -4639,7 +4634,7 @@
       <c r="B180" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C180" s="3" t="n">
+      <c r="C180" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D180" s="1" t="s">
@@ -4659,7 +4654,7 @@
       <c r="B181" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C181" s="3" t="n">
+      <c r="C181" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D181" s="1" t="s">
@@ -4676,7 +4671,7 @@
       <c r="B182" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C182" s="3" t="n">
+      <c r="C182" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D182" s="1" t="s">
@@ -4696,7 +4691,7 @@
       <c r="B183" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C183" s="3" t="n">
+      <c r="C183" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D183" s="1" t="s">
@@ -4716,7 +4711,7 @@
       <c r="B184" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C184" s="3" t="n">
+      <c r="C184" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D184" s="1" t="s">
@@ -4742,7 +4737,7 @@
       <c r="B185" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C185" s="3" t="n">
+      <c r="C185" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D185" s="1" t="s">
@@ -4768,7 +4763,7 @@
       <c r="B186" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C186" s="3" t="n">
+      <c r="C186" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D186" s="1" t="s">
@@ -4794,7 +4789,7 @@
       <c r="B187" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C187" s="3" t="n">
+      <c r="C187" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D187" s="1" t="s">
@@ -4820,7 +4815,7 @@
       <c r="B188" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C188" s="3" t="n">
+      <c r="C188" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D188" s="1" t="s">
@@ -4846,7 +4841,7 @@
       <c r="B189" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C189" s="3" t="n">
+      <c r="C189" s="2" t="n">
         <v>44202</v>
       </c>
       <c r="D189" s="1" t="s">

</xml_diff>